<commit_message>
Started big complicated match events download.
</commit_message>
<xml_diff>
--- a/Opta.xlsx
+++ b/Opta.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="69">
   <si>
     <t xml:space="preserve">Table</t>
   </si>
@@ -224,6 +224,9 @@
   </si>
   <si>
     <t xml:space="preserve">PlayersDownloaded</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Summary…</t>
   </si>
 </sst>
 </file>
@@ -475,17 +478,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C68"/>
+  <dimension ref="A1:C69"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A50" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A70" activeCellId="0" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="22.4081632653061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="69.7908163265306"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="68.9795918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1033,6 +1036,11 @@
       </c>
       <c r="B68" s="4" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>